<commit_message>
Modified frmAddUser to correct bindingsources of controls
</commit_message>
<xml_diff>
--- a/Documents/Things to Update on GUI.xlsx
+++ b/Documents/Things to Update on GUI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yura\Documents\Projects\Laboratory Asset Inventory\LabAssetInventory\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yura\Documents\Projects\PNGIMR_IS\PNGIMR_IS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>27/07/23</t>
+  </si>
+  <si>
+    <t>25/08/2023</t>
+  </si>
+  <si>
+    <t>grid data is not shown on controls esp textboxes</t>
   </si>
 </sst>
 </file>
@@ -553,7 +559,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,9 +876,15 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="17"/>
+      <c r="A24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>40</v>
+      </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed database name from pngimr_lab_inventory to PNGIMR_IS
</commit_message>
<xml_diff>
--- a/Documents/Things to Update on GUI.xlsx
+++ b/Documents/Things to Update on GUI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>grid data is not shown on controls esp textboxes</t>
+  </si>
+  <si>
+    <t>25/08/23</t>
+  </si>
+  <si>
+    <t>password displayed on the control should not show the characters</t>
   </si>
 </sst>
 </file>
@@ -559,7 +565,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,21 +882,29 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="17"/>
+      <c r="A25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change first letters of methods and variables from lowercase to uppercases
</commit_message>
<xml_diff>
--- a/Documents/Things to Update on GUI.xlsx
+++ b/Documents/Things to Update on GUI.xlsx
@@ -236,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -281,6 +281,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,7 +568,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,16 +899,18 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="19">
+        <v>45055</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>

</xml_diff>

<commit_message>
added a test code to load event of form login
</commit_message>
<xml_diff>
--- a/Documents/Things to Update on GUI.xlsx
+++ b/Documents/Things to Update on GUI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>password displayed on the control should not show the characters</t>
+  </si>
+  <si>
+    <t>Change control asset name field from textbox to combobox</t>
+  </si>
+  <si>
+    <t>Change control brand field from textbox to combobox</t>
+  </si>
+  <si>
+    <t>Change control category field from textbox to combobox</t>
   </si>
 </sst>
 </file>
@@ -236,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -283,6 +292,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -567,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,21 +925,39 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="17"/>
+      <c r="A26" s="20">
+        <v>45055</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="17"/>
+      <c r="A27" s="20">
+        <v>45055</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>44</v>
+      </c>
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="17"/>
+      <c r="A28" s="20">
+        <v>45055</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>